<commit_message>
3e vorm met correcte LijktOp kolom
</commit_message>
<xml_diff>
--- a/NetflixStatistics/SQL Database/3e vorm.xlsx
+++ b/NetflixStatistics/SQL Database/3e vorm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\Desktop\Avans\Periode 2\Databases 2\SQL Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E405D2A-D625-4505-B043-CC52FA5D7F06}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60D67BB5-ECDB-424F-9B5F-983DDA739873}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{ACF3DB3C-4AA0-41F9-8FE3-9C7617583530}"/>
+    <workbookView xWindow="3048" yWindow="4080" windowWidth="17304" windowHeight="12360" firstSheet="3" activeTab="5" xr2:uid="{ACF3DB3C-4AA0-41F9-8FE3-9C7617583530}"/>
   </bookViews>
   <sheets>
     <sheet name="Accounts" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="124">
   <si>
     <t>Naam</t>
   </si>
@@ -331,12 +331,6 @@
     <t>A Clockwork Orange</t>
   </si>
   <si>
-    <t>5 Days Out</t>
-  </si>
-  <si>
-    <t>6 Days Out</t>
-  </si>
-  <si>
     <t>Genre</t>
   </si>
   <si>
@@ -352,9 +346,6 @@
     <t>Engels</t>
   </si>
   <si>
-    <t>&gt;12</t>
-  </si>
-  <si>
     <t>Humor</t>
   </si>
   <si>
@@ -373,12 +364,6 @@
     <t>Nederlands</t>
   </si>
   <si>
-    <t>&gt;16</t>
-  </si>
-  <si>
-    <t>&gt;18</t>
-  </si>
-  <si>
     <t>Oorlog</t>
   </si>
   <si>
@@ -391,9 +376,6 @@
     <t>Vlaams</t>
   </si>
   <si>
-    <t>&gt;6</t>
-  </si>
-  <si>
     <t>Spanning</t>
   </si>
   <si>
@@ -416,6 +398,18 @@
   </si>
   <si>
     <t>Seizoen ID</t>
+  </si>
+  <si>
+    <t>LijktOp</t>
+  </si>
+  <si>
+    <t>Sherlock</t>
+  </si>
+  <si>
+    <t>Breaking Bad</t>
+  </si>
+  <si>
+    <t>Fargo</t>
   </si>
 </sst>
 </file>
@@ -644,7 +638,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -679,10 +673,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -800,13 +791,15 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{27CF0914-6DCE-4826-84A0-CA9CBC3AEBE2}" name="Tabel5" displayName="Tabel5" ref="B2:E6" totalsRowShown="0">
-  <autoFilter ref="B2:E6" xr:uid="{F74FAAD3-0EEE-453B-96ED-11D878C80B09}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{27CF0914-6DCE-4826-84A0-CA9CBC3AEBE2}" name="Tabel5" displayName="Tabel5" ref="B2:G5" totalsRowShown="0">
+  <autoFilter ref="B2:G5" xr:uid="{F74FAAD3-0EEE-453B-96ED-11D878C80B09}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{260AEF99-A0BE-4970-BE1F-0722055E9F16}" name="Serie ID"/>
     <tableColumn id="2" xr3:uid="{39DF9974-4652-4F88-9ACD-EF0FC13926D1}" name="Genre"/>
     <tableColumn id="3" xr3:uid="{BBBB0E26-0E74-4848-8840-1867CA8B0208}" name="Taal"/>
     <tableColumn id="4" xr3:uid="{6D4F8378-45B9-43E3-96CC-6B0AB3EFB82D}" name="Leeftijdsindicatie"/>
+    <tableColumn id="5" xr3:uid="{8BDCB700-FE54-402F-969E-CD9777CE7DBE}" name="Naam"/>
+    <tableColumn id="6" xr3:uid="{8AAFBB7E-BF18-4C97-B511-18C64257ABA5}" name="LijktOp"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1258,7 +1251,7 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
@@ -1462,10 +1455,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{637D77A6-5D13-42E4-9C7D-EED1D25CD03B}">
-  <dimension ref="A1:C64"/>
+  <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1477,7 +1470,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>34</v>
@@ -1774,10 +1767,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="26">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="B28" s="27" t="s">
-        <v>97</v>
+        <v>63</v>
       </c>
       <c r="C28" s="18">
         <v>48</v>
@@ -1785,10 +1778,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="24">
-        <v>2015</v>
+        <v>2017</v>
       </c>
       <c r="B29" s="25" t="s">
-        <v>98</v>
+        <v>64</v>
       </c>
       <c r="C29" s="19">
         <v>48</v>
@@ -1796,10 +1789,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="26">
-        <v>2016</v>
+        <v>2018</v>
       </c>
       <c r="B30" s="27" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C30" s="18">
         <v>48</v>
@@ -1807,10 +1800,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="24">
-        <v>2017</v>
+        <v>2019</v>
       </c>
       <c r="B31" s="25" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C31" s="19">
         <v>48</v>
@@ -1818,32 +1811,32 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="26">
-        <v>2018</v>
-      </c>
-      <c r="B32" s="27" t="s">
-        <v>65</v>
+        <v>3001</v>
+      </c>
+      <c r="B32" s="33" t="s">
+        <v>67</v>
       </c>
       <c r="C32" s="18">
-        <v>48</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="24">
-        <v>2019</v>
-      </c>
-      <c r="B33" s="25" t="s">
-        <v>66</v>
+        <v>3002</v>
+      </c>
+      <c r="B33" s="32" t="s">
+        <v>68</v>
       </c>
       <c r="C33" s="19">
-        <v>48</v>
+        <v>68</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="26">
-        <v>3001</v>
+        <v>3003</v>
       </c>
       <c r="B34" s="33" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C34" s="18">
         <v>68</v>
@@ -1851,10 +1844,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="24">
-        <v>3002</v>
+        <v>3004</v>
       </c>
       <c r="B35" s="32" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C35" s="19">
         <v>68</v>
@@ -1862,10 +1855,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="26">
-        <v>3003</v>
+        <v>3005</v>
       </c>
       <c r="B36" s="33" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C36" s="18">
         <v>68</v>
@@ -1873,10 +1866,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="24">
-        <v>3004</v>
+        <v>3006</v>
       </c>
       <c r="B37" s="32" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C37" s="19">
         <v>68</v>
@@ -1884,10 +1877,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="26">
-        <v>3005</v>
+        <v>3007</v>
       </c>
       <c r="B38" s="33" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C38" s="18">
         <v>68</v>
@@ -1895,10 +1888,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="24">
-        <v>3006</v>
+        <v>3008</v>
       </c>
       <c r="B39" s="32" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C39" s="19">
         <v>68</v>
@@ -1906,10 +1899,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="26">
-        <v>3007</v>
+        <v>3009</v>
       </c>
       <c r="B40" s="33" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C40" s="18">
         <v>68</v>
@@ -1917,10 +1910,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="24">
-        <v>3008</v>
+        <v>3010</v>
       </c>
       <c r="B41" s="32" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C41" s="19">
         <v>68</v>
@@ -1928,98 +1921,98 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="26">
-        <v>3009</v>
+        <v>8001</v>
       </c>
       <c r="B42" s="33" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C42" s="18">
-        <v>68</v>
+        <v>94</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="24">
-        <v>3010</v>
-      </c>
-      <c r="B43" s="32" t="s">
-        <v>76</v>
-      </c>
-      <c r="C43" s="19">
-        <v>68</v>
+      <c r="A43" s="26">
+        <v>8002</v>
+      </c>
+      <c r="B43" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="C43" s="18">
+        <v>154</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="26">
-        <v>8001</v>
+        <v>8004</v>
       </c>
       <c r="B44" s="33" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C44" s="18">
-        <v>94</v>
+        <v>80</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="26">
-        <v>8002</v>
+        <v>8008</v>
       </c>
       <c r="B45" s="33" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C45" s="18">
-        <v>154</v>
+        <v>99</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="26">
-        <v>8004</v>
-      </c>
-      <c r="B46" s="33" t="s">
-        <v>79</v>
-      </c>
-      <c r="C46" s="18">
-        <v>80</v>
+      <c r="A46" s="24">
+        <v>8010</v>
+      </c>
+      <c r="B46" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="C46" s="19">
+        <v>161</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="26">
-        <v>8008</v>
+        <v>8011</v>
       </c>
       <c r="B47" s="33" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C47" s="18">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="24">
-        <v>8010</v>
-      </c>
-      <c r="B48" s="32" t="s">
-        <v>81</v>
+        <v>3101</v>
+      </c>
+      <c r="B48" s="34" t="s">
+        <v>83</v>
       </c>
       <c r="C48" s="19">
-        <v>161</v>
+        <v>68</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="26">
-        <v>8011</v>
-      </c>
-      <c r="B49" s="33" t="s">
-        <v>82</v>
+        <v>3102</v>
+      </c>
+      <c r="B49" s="27" t="s">
+        <v>84</v>
       </c>
       <c r="C49" s="18">
-        <v>103</v>
+        <v>68</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="24">
-        <v>3101</v>
-      </c>
-      <c r="B50" s="35" t="s">
-        <v>83</v>
+        <v>3103</v>
+      </c>
+      <c r="B50" s="25" t="s">
+        <v>85</v>
       </c>
       <c r="C50" s="19">
         <v>68</v>
@@ -2027,10 +2020,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="26">
-        <v>3102</v>
+        <v>3105</v>
       </c>
       <c r="B51" s="27" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C51" s="18">
         <v>68</v>
@@ -2038,10 +2031,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="24">
-        <v>3103</v>
+        <v>3104</v>
       </c>
       <c r="B52" s="25" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C52" s="19">
         <v>68</v>
@@ -2049,10 +2042,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="26">
-        <v>3105</v>
+        <v>3106</v>
       </c>
       <c r="B53" s="27" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C53" s="18">
         <v>68</v>
@@ -2060,10 +2053,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="24">
-        <v>3104</v>
+        <v>3107</v>
       </c>
       <c r="B54" s="25" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C54" s="19">
         <v>68</v>
@@ -2071,10 +2064,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="26">
-        <v>3106</v>
+        <v>3108</v>
       </c>
       <c r="B55" s="27" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C55" s="18">
         <v>68</v>
@@ -2082,10 +2075,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="24">
-        <v>3107</v>
+        <v>3109</v>
       </c>
       <c r="B56" s="25" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C56" s="19">
         <v>68</v>
@@ -2093,10 +2086,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="26">
-        <v>3108</v>
+        <v>3110</v>
       </c>
       <c r="B57" s="27" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C57" s="18">
         <v>68</v>
@@ -2104,74 +2097,47 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="24">
-        <v>3109</v>
+        <v>8012</v>
       </c>
       <c r="B58" s="25" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C58" s="19">
-        <v>68</v>
+        <v>97</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="26">
-        <v>3110</v>
+        <v>8014</v>
       </c>
       <c r="B59" s="27" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C59" s="18">
-        <v>68</v>
+        <v>178</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="24">
-        <v>8012</v>
+        <v>8016</v>
       </c>
       <c r="B60" s="25" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C60" s="19">
-        <v>97</v>
+        <v>108</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="26">
-        <v>8014</v>
+        <v>8017</v>
       </c>
       <c r="B61" s="27" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C61" s="18">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A62" s="24">
-        <v>8016</v>
-      </c>
-      <c r="B62" s="25" t="s">
-        <v>95</v>
-      </c>
-      <c r="C62" s="19">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A63" s="26">
-        <v>8017</v>
-      </c>
-      <c r="B63" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="C63" s="18">
         <v>136</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A64" s="34"/>
-      <c r="B64" s="36"/>
-      <c r="C64" s="37"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2182,7 +2148,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5853E1E-6576-42D4-B934-E3EA5212DE8A}">
   <dimension ref="B2:G183"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
@@ -2198,7 +2164,7 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C2" t="s">
         <v>36</v>
@@ -2207,7 +2173,7 @@
         <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
@@ -4759,7 +4725,7 @@
   <dimension ref="B2:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4771,16 +4737,16 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E2" t="s">
         <v>99</v>
-      </c>
-      <c r="D2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E2" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
@@ -4788,13 +4754,13 @@
         <v>1010</v>
       </c>
       <c r="C3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D3" t="s">
-        <v>103</v>
-      </c>
-      <c r="E3" t="s">
-        <v>104</v>
+        <v>101</v>
+      </c>
+      <c r="E3">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
@@ -4802,13 +4768,13 @@
         <v>8001</v>
       </c>
       <c r="C4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D4" t="s">
-        <v>103</v>
-      </c>
-      <c r="E4" t="s">
-        <v>104</v>
+        <v>101</v>
+      </c>
+      <c r="E4">
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
@@ -4816,13 +4782,13 @@
         <v>8002</v>
       </c>
       <c r="C5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" t="s">
         <v>106</v>
       </c>
-      <c r="D5" t="s">
-        <v>109</v>
-      </c>
-      <c r="E5" t="s">
-        <v>111</v>
+      <c r="E5">
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
@@ -4830,13 +4796,13 @@
         <v>8004</v>
       </c>
       <c r="C6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" t="s">
         <v>107</v>
       </c>
-      <c r="D6" t="s">
-        <v>110</v>
-      </c>
-      <c r="E6" t="s">
-        <v>112</v>
+      <c r="E6">
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.3">
@@ -4844,13 +4810,13 @@
         <v>8008</v>
       </c>
       <c r="C7" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7" t="s">
         <v>106</v>
       </c>
-      <c r="D7" t="s">
-        <v>109</v>
-      </c>
-      <c r="E7" t="s">
-        <v>111</v>
+      <c r="E7">
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.3">
@@ -4858,13 +4824,13 @@
         <v>8010</v>
       </c>
       <c r="C8" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="E8" t="s">
-        <v>104</v>
+        <v>106</v>
+      </c>
+      <c r="E8">
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.3">
@@ -4872,13 +4838,13 @@
         <v>8011</v>
       </c>
       <c r="C9" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="E9" t="s">
-        <v>111</v>
+        <v>106</v>
+      </c>
+      <c r="E9">
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.3">
@@ -4886,13 +4852,13 @@
         <v>8012</v>
       </c>
       <c r="C10" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D10" t="s">
-        <v>110</v>
-      </c>
-      <c r="E10" t="s">
-        <v>117</v>
+        <v>107</v>
+      </c>
+      <c r="E10">
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.3">
@@ -4900,13 +4866,13 @@
         <v>8014</v>
       </c>
       <c r="C11" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D11" t="s">
-        <v>115</v>
-      </c>
-      <c r="E11" t="s">
-        <v>117</v>
+        <v>110</v>
+      </c>
+      <c r="E11">
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
@@ -4914,13 +4880,13 @@
         <v>8016</v>
       </c>
       <c r="C12" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D12" t="s">
-        <v>116</v>
-      </c>
-      <c r="E12" t="s">
-        <v>104</v>
+        <v>111</v>
+      </c>
+      <c r="E12">
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.3">
@@ -4928,13 +4894,13 @@
         <v>8017</v>
       </c>
       <c r="C13" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D13" t="s">
-        <v>103</v>
-      </c>
-      <c r="E13" t="s">
-        <v>111</v>
+        <v>101</v>
+      </c>
+      <c r="E13">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -4947,86 +4913,97 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE7FFF3C-3BB4-4D22-BE30-5E2A778286DB}">
-  <dimension ref="B2:E6"/>
+  <dimension ref="B2:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.109375" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E2" t="s">
         <v>99</v>
       </c>
-      <c r="D2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D3" t="s">
-        <v>103</v>
-      </c>
-      <c r="E3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E3">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>121</v>
+      </c>
+      <c r="G3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D4" t="s">
-        <v>109</v>
-      </c>
-      <c r="E4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+      <c r="E4">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>122</v>
+      </c>
+      <c r="G4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="E5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>118</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="E6" t="s">
-        <v>111</v>
+        <v>106</v>
+      </c>
+      <c r="E5">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G5" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -5042,7 +5019,7 @@
   <dimension ref="B2:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5054,16 +5031,16 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="C2" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="E2" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
@@ -5155,7 +5132,7 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9">
         <v>10</v>
@@ -5176,8 +5153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70848D41-AC78-4B9A-A614-C4FB5196F496}">
   <dimension ref="B2:D51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5189,13 +5166,13 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C2" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D2" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">

</xml_diff>